<commit_message>
Now using iQp, iXp, iQf, and iXf. p and f denote primary and final.
</commit_message>
<xml_diff>
--- a/data/Excel Workbooks/Calvin/ChinaDataWorkbook.xlsx
+++ b/data/Excel Workbooks/Calvin/ChinaDataWorkbook.xlsx
@@ -23,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="133">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="201" uniqueCount="135">
   <si>
     <t>Exergy [TJ]</t>
   </si>
@@ -956,6 +956,12 @@
   </si>
   <si>
     <t>Calvin</t>
+  </si>
+  <si>
+    <t>iQp</t>
+  </si>
+  <si>
+    <t>iXp</t>
   </si>
 </sst>
 </file>
@@ -2617,6 +2623,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="18" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="21" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -2627,9 +2636,6 @@
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="18" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
@@ -3987,11 +3993,11 @@
           <c:showPercent val="0"/>
           <c:showBubbleSize val="0"/>
         </c:dLbls>
-        <c:axId val="2094843864"/>
-        <c:axId val="-2115353128"/>
+        <c:axId val="2103806184"/>
+        <c:axId val="2101239016"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="2094843864"/>
+        <c:axId val="2103806184"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4013,7 +4019,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="General" sourceLinked="1"/>
@@ -4030,12 +4035,12 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="-2115353128"/>
+        <c:crossAx val="2101239016"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="-2115353128"/>
+        <c:axId val="2101239016"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -4057,7 +4062,6 @@
               </a:p>
             </c:rich>
           </c:tx>
-          <c:layout/>
           <c:overlay val="0"/>
         </c:title>
         <c:numFmt formatCode="0" sourceLinked="0"/>
@@ -4074,7 +4078,7 @@
             <a:endParaRPr lang="en-US"/>
           </a:p>
         </c:txPr>
-        <c:crossAx val="2094843864"/>
+        <c:crossAx val="2103806184"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -6213,7 +6217,7 @@
   <dimension ref="A1:J22"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2:J22"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="14" x14ac:dyDescent="0"/>
@@ -6240,13 +6244,11 @@
       <c r="E1" s="76" t="s">
         <v>130</v>
       </c>
-      <c r="F1" s="76" t="str">
-        <f>'China Workbook'!K9</f>
-        <v>iQ</v>
-      </c>
-      <c r="G1" s="76" t="str">
-        <f>'China Workbook'!L9</f>
-        <v>iX</v>
+      <c r="F1" s="76" t="s">
+        <v>133</v>
+      </c>
+      <c r="G1" s="76" t="s">
+        <v>134</v>
       </c>
       <c r="H1" s="21" t="s">
         <v>112</v>
@@ -8421,13 +8423,13 @@
       </c>
     </row>
     <row r="29" spans="1:41" ht="15" customHeight="1">
-      <c r="A29" s="100" t="s">
+      <c r="A29" s="101" t="s">
         <v>1</v>
       </c>
       <c r="B29" s="96" t="s">
         <v>23</v>
       </c>
-      <c r="C29" s="102" t="s">
+      <c r="C29" s="103" t="s">
         <v>24</v>
       </c>
       <c r="D29" s="96" t="s">
@@ -8460,10 +8462,10 @@
       <c r="M29" s="98" t="s">
         <v>74</v>
       </c>
-      <c r="N29" s="100" t="s">
+      <c r="N29" s="101" t="s">
         <v>61</v>
       </c>
-      <c r="O29" s="102" t="s">
+      <c r="O29" s="103" t="s">
         <v>62</v>
       </c>
       <c r="P29" s="96" t="s">
@@ -8478,10 +8480,10 @@
       <c r="S29" s="96" t="s">
         <v>85</v>
       </c>
-      <c r="T29" s="100" t="s">
+      <c r="T29" s="101" t="s">
         <v>27</v>
       </c>
-      <c r="U29" s="102" t="s">
+      <c r="U29" s="103" t="s">
         <v>28</v>
       </c>
       <c r="V29" s="96" t="s">
@@ -8511,10 +8513,10 @@
       <c r="AD29" s="98" t="s">
         <v>32</v>
       </c>
-      <c r="AE29" s="100" t="s">
+      <c r="AE29" s="101" t="s">
         <v>87</v>
       </c>
-      <c r="AF29" s="102" t="s">
+      <c r="AF29" s="103" t="s">
         <v>88</v>
       </c>
       <c r="AG29" s="96" t="s">
@@ -8546,9 +8548,9 @@
       </c>
     </row>
     <row r="30" spans="1:41">
-      <c r="A30" s="101"/>
+      <c r="A30" s="102"/>
       <c r="B30" s="97"/>
-      <c r="C30" s="103"/>
+      <c r="C30" s="104"/>
       <c r="D30" s="97"/>
       <c r="E30" s="97"/>
       <c r="F30" s="97"/>
@@ -8558,15 +8560,15 @@
       <c r="J30" s="97"/>
       <c r="K30" s="97"/>
       <c r="L30" s="97"/>
-      <c r="M30" s="104"/>
-      <c r="N30" s="101"/>
-      <c r="O30" s="103"/>
+      <c r="M30" s="100"/>
+      <c r="N30" s="102"/>
+      <c r="O30" s="104"/>
       <c r="P30" s="97"/>
       <c r="Q30" s="97"/>
       <c r="R30" s="97"/>
       <c r="S30" s="97"/>
-      <c r="T30" s="101"/>
-      <c r="U30" s="103"/>
+      <c r="T30" s="102"/>
+      <c r="U30" s="104"/>
       <c r="V30" s="97"/>
       <c r="W30" s="97"/>
       <c r="X30" s="97"/>
@@ -8576,8 +8578,8 @@
       <c r="AB30" s="97"/>
       <c r="AC30" s="97"/>
       <c r="AD30" s="99"/>
-      <c r="AE30" s="101"/>
-      <c r="AF30" s="103"/>
+      <c r="AE30" s="102"/>
+      <c r="AF30" s="104"/>
       <c r="AG30" s="97"/>
       <c r="AH30" s="97"/>
       <c r="AI30" s="97"/>
@@ -13304,15 +13306,26 @@
     </row>
   </sheetData>
   <mergeCells count="41">
-    <mergeCell ref="Z29:Z30"/>
-    <mergeCell ref="AA29:AA30"/>
-    <mergeCell ref="AK29:AK30"/>
-    <mergeCell ref="AL29:AL30"/>
-    <mergeCell ref="Y29:Y30"/>
-    <mergeCell ref="AB29:AB30"/>
-    <mergeCell ref="AC29:AC30"/>
-    <mergeCell ref="AD29:AD30"/>
-    <mergeCell ref="AJ29:AJ30"/>
+    <mergeCell ref="AM29:AM30"/>
+    <mergeCell ref="AN29:AN30"/>
+    <mergeCell ref="AO29:AO30"/>
+    <mergeCell ref="AE29:AE30"/>
+    <mergeCell ref="AF29:AF30"/>
+    <mergeCell ref="AG29:AG30"/>
+    <mergeCell ref="AH29:AH30"/>
+    <mergeCell ref="AI29:AI30"/>
+    <mergeCell ref="A29:A30"/>
+    <mergeCell ref="B29:B30"/>
+    <mergeCell ref="C29:C30"/>
+    <mergeCell ref="D29:D30"/>
+    <mergeCell ref="E29:E30"/>
+    <mergeCell ref="F29:F30"/>
+    <mergeCell ref="G29:G30"/>
+    <mergeCell ref="H29:H30"/>
+    <mergeCell ref="I29:I30"/>
+    <mergeCell ref="L29:L30"/>
+    <mergeCell ref="J29:J30"/>
+    <mergeCell ref="K29:K30"/>
     <mergeCell ref="M29:M30"/>
     <mergeCell ref="X29:X30"/>
     <mergeCell ref="N29:N30"/>
@@ -13325,26 +13338,15 @@
     <mergeCell ref="W29:W30"/>
     <mergeCell ref="Q29:Q30"/>
     <mergeCell ref="R29:R30"/>
-    <mergeCell ref="F29:F30"/>
-    <mergeCell ref="G29:G30"/>
-    <mergeCell ref="H29:H30"/>
-    <mergeCell ref="I29:I30"/>
-    <mergeCell ref="L29:L30"/>
-    <mergeCell ref="J29:J30"/>
-    <mergeCell ref="K29:K30"/>
-    <mergeCell ref="A29:A30"/>
-    <mergeCell ref="B29:B30"/>
-    <mergeCell ref="C29:C30"/>
-    <mergeCell ref="D29:D30"/>
-    <mergeCell ref="E29:E30"/>
-    <mergeCell ref="AM29:AM30"/>
-    <mergeCell ref="AN29:AN30"/>
-    <mergeCell ref="AO29:AO30"/>
-    <mergeCell ref="AE29:AE30"/>
-    <mergeCell ref="AF29:AF30"/>
-    <mergeCell ref="AG29:AG30"/>
-    <mergeCell ref="AH29:AH30"/>
-    <mergeCell ref="AI29:AI30"/>
+    <mergeCell ref="Z29:Z30"/>
+    <mergeCell ref="AA29:AA30"/>
+    <mergeCell ref="AK29:AK30"/>
+    <mergeCell ref="AL29:AL30"/>
+    <mergeCell ref="Y29:Y30"/>
+    <mergeCell ref="AB29:AB30"/>
+    <mergeCell ref="AC29:AC30"/>
+    <mergeCell ref="AD29:AD30"/>
+    <mergeCell ref="AJ29:AJ30"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <extLst>

</xml_diff>